<commit_message>
added logic for identifying test suite and test case runmode
</commit_message>
<xml_diff>
--- a/src/test/resources/testdata/BankManagerSuite.xlsx
+++ b/src/test/resources/testdata/BankManagerSuite.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Manish_Katepallewar\eclipse-workspace\TestDataProject\src\test\resources\testdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FBC0CC3B-353D-45A6-9410-706016827D1E}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7FB8ED1F-5B48-4AF2-9289-C7FF14598BE4}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="915" yWindow="-120" windowWidth="28005" windowHeight="16440" activeTab="1" xr2:uid="{649B13FE-0F32-45E6-A09F-C23029F507DA}"/>
+    <workbookView xWindow="39150" yWindow="3000" windowWidth="20820" windowHeight="11835" xr2:uid="{649B13FE-0F32-45E6-A09F-C23029F507DA}"/>
   </bookViews>
   <sheets>
     <sheet name="TestCases" sheetId="1" r:id="rId1"/>
@@ -445,8 +445,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{15A26B2B-C290-4CD6-AC1F-130AC29407C7}">
   <dimension ref="A1:B3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -488,7 +488,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C78939DD-E20B-419D-B45B-DFA0009D20C1}">
   <dimension ref="A1:D9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
added paratemerisation and hashtable for data reading
</commit_message>
<xml_diff>
--- a/src/test/resources/testdata/BankManagerSuite.xlsx
+++ b/src/test/resources/testdata/BankManagerSuite.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Manish_Katepallewar\eclipse-workspace\TestDataProject\src\test\resources\testdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7FB8ED1F-5B48-4AF2-9289-C7FF14598BE4}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BAAC196C-AE18-4F69-86E5-696D6CA42F36}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="39150" yWindow="3000" windowWidth="20820" windowHeight="11835" xr2:uid="{649B13FE-0F32-45E6-A09F-C23029F507DA}"/>
+    <workbookView minimized="1" xWindow="36780" yWindow="3000" windowWidth="20820" windowHeight="11835" activeTab="1" xr2:uid="{649B13FE-0F32-45E6-A09F-C23029F507DA}"/>
   </bookViews>
   <sheets>
     <sheet name="TestCases" sheetId="1" r:id="rId1"/>
@@ -445,7 +445,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{15A26B2B-C290-4CD6-AC1F-130AC29407C7}">
   <dimension ref="A1:B3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
@@ -488,9 +488,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C78939DD-E20B-419D-B45B-DFA0009D20C1}">
   <dimension ref="A1:D9"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>

</xml_diff>

<commit_message>
Optimize dataprovider class and added test cases for bankmanager
</commit_message>
<xml_diff>
--- a/src/test/resources/testdata/BankManagerSuite.xlsx
+++ b/src/test/resources/testdata/BankManagerSuite.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Manish_Katepallewar\eclipse-workspace\TestDataProject\src\test\resources\testdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BAAC196C-AE18-4F69-86E5-696D6CA42F36}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AB2D507B-4298-4407-A229-7FBEA8E942EF}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView minimized="1" xWindow="36780" yWindow="3000" windowWidth="20820" windowHeight="11835" activeTab="1" xr2:uid="{649B13FE-0F32-45E6-A09F-C23029F507DA}"/>
+    <workbookView xWindow="36780" yWindow="3000" windowWidth="20820" windowHeight="11835" activeTab="1" xr2:uid="{649B13FE-0F32-45E6-A09F-C23029F507DA}"/>
   </bookViews>
   <sheets>
     <sheet name="TestCases" sheetId="1" r:id="rId1"/>
@@ -488,7 +488,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C78939DD-E20B-419D-B45B-DFA0009D20C1}">
   <dimension ref="A1:D9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A6" sqref="A6"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>

</xml_diff>

<commit_message>
added common utility for runmodes
</commit_message>
<xml_diff>
--- a/src/test/resources/testdata/BankManagerSuite.xlsx
+++ b/src/test/resources/testdata/BankManagerSuite.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Manish_Katepallewar\eclipse-workspace\TestDataProject\src\test\resources\testdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AB2D507B-4298-4407-A229-7FBEA8E942EF}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{14BF0155-05A9-4001-BA4B-92B87B8240D9}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="36780" yWindow="3000" windowWidth="20820" windowHeight="11835" activeTab="1" xr2:uid="{649B13FE-0F32-45E6-A09F-C23029F507DA}"/>
+    <workbookView xWindow="2115" yWindow="1080" windowWidth="20820" windowHeight="11835" xr2:uid="{649B13FE-0F32-45E6-A09F-C23029F507DA}"/>
   </bookViews>
   <sheets>
     <sheet name="TestCases" sheetId="1" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="20">
   <si>
     <t>TestCases</t>
   </si>
@@ -445,8 +445,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{15A26B2B-C290-4CD6-AC1F-130AC29407C7}">
   <dimension ref="A1:B3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -476,7 +476,7 @@
         <v>3</v>
       </c>
       <c r="B3" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
   </sheetData>
@@ -486,10 +486,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C78939DD-E20B-419D-B45B-DFA0009D20C1}">
-  <dimension ref="A1:D9"/>
+  <dimension ref="A1:D13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A13" sqref="A13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -529,7 +529,7 @@
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B4" t="s">
         <v>16</v>
@@ -541,41 +541,91 @@
         <v>12</v>
       </c>
     </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>4</v>
+      </c>
+      <c r="B5" t="s">
+        <v>9</v>
+      </c>
+      <c r="C5" t="s">
+        <v>10</v>
+      </c>
+      <c r="D5" t="s">
+        <v>11</v>
+      </c>
+    </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>1</v>
-      </c>
-      <c r="B7" t="s">
-        <v>13</v>
-      </c>
-      <c r="C7" t="s">
-        <v>14</v>
+        <v>4</v>
+      </c>
+      <c r="B6" t="s">
+        <v>16</v>
+      </c>
+      <c r="C6" t="s">
+        <v>10</v>
+      </c>
+      <c r="D6" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>4</v>
-      </c>
-      <c r="B8" t="s">
-        <v>15</v>
-      </c>
-      <c r="C8" t="s">
-        <v>18</v>
+        <v>3</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="B9" t="s">
+        <v>13</v>
+      </c>
+      <c r="C9" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>4</v>
+      </c>
+      <c r="B10" t="s">
+        <v>15</v>
+      </c>
+      <c r="C10" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>5</v>
+      </c>
+      <c r="B11" t="s">
         <v>17</v>
       </c>
-      <c r="C9" t="s">
+      <c r="C11" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>4</v>
+      </c>
+      <c r="B12" t="s">
+        <v>15</v>
+      </c>
+      <c r="C12" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>5</v>
+      </c>
+      <c r="B13" t="s">
+        <v>17</v>
+      </c>
+      <c r="C13" t="s">
         <v>19</v>
       </c>
     </row>

</xml_diff>